<commit_message>
Some notes on custom monster card types, and with it, notes for Elemental HERO retrains / missing Fusion Monsters.
</commit_message>
<xml_diff>
--- a/Custom Cards/Format - 2014-07 HAT/Elemental HERO/Classic Elemental HERO Combinations.xlsx
+++ b/Custom Cards/Format - 2014-07 HAT/Elemental HERO/Classic Elemental HERO Combinations.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\Format - 2008-07 Gladiator\Elemental HERO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\Format - 2014-07 HAT\Elemental HERO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EED8C82-2C5A-4E88-B6A4-E25A730B58F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769FBD4E-3F0F-45FC-978E-713FB2DA1F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2ED25532-7934-4E3F-8319-AC4FDB9A5A39}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{2ED25532-7934-4E3F-8319-AC4FDB9A5A39}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="127">
   <si>
     <t>Avian</t>
   </si>
@@ -138,9 +140,6 @@
     <t>Tombstone</t>
   </si>
   <si>
-    <t>Ceramic Edge</t>
-  </si>
-  <si>
     <t>Forge</t>
   </si>
   <si>
@@ -178,13 +177,244 @@
   </si>
   <si>
     <t>METAL?</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Rock</t>
+  </si>
+  <si>
+    <t>Aqua</t>
+  </si>
+  <si>
+    <t>Pyro</t>
+  </si>
+  <si>
+    <t>Air</t>
+  </si>
+  <si>
+    <t>Thunder</t>
+  </si>
+  <si>
+    <t>Shadow</t>
+  </si>
+  <si>
+    <t>Plant</t>
+  </si>
+  <si>
+    <t>Metal</t>
+  </si>
+  <si>
+    <t>Anime</t>
+  </si>
+  <si>
+    <t>Manga</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Knopse Poison Rose Woodsman</t>
+  </si>
+  <si>
+    <t>Liquid Soldier</t>
+  </si>
+  <si>
+    <t>Ice Edge      Ocean</t>
+  </si>
+  <si>
+    <t>Captain Gold Solid Soldier</t>
+  </si>
+  <si>
+    <t>Heat                Lady Heat</t>
+  </si>
+  <si>
+    <t>Blazeman</t>
+  </si>
+  <si>
+    <t>Stratos</t>
+  </si>
+  <si>
+    <t>Neos</t>
+  </si>
+  <si>
+    <t>Clayman Prisma</t>
+  </si>
+  <si>
+    <t>Flash Voltic</t>
+  </si>
+  <si>
+    <t>Neos Alius        Honest Neos         Spirit of Neos Winged Kuriboh LV6</t>
+  </si>
+  <si>
+    <t>Shadow Mist</t>
+  </si>
+  <si>
+    <t>Alloy</t>
+  </si>
+  <si>
+    <t>Own effects</t>
+  </si>
+  <si>
+    <t>Common effects for Fusion Monsters</t>
+  </si>
+  <si>
+    <t>Piercing, monster destruction</t>
+  </si>
+  <si>
+    <t>Easier attacks</t>
+  </si>
+  <si>
+    <t>GY interaction</t>
+  </si>
+  <si>
+    <t>Easy damage, low-ish ATK</t>
+  </si>
+  <si>
+    <t>Low ATK, LP difference (easy damage, heal)</t>
+  </si>
+  <si>
+    <t>LP difference (easy / bonus damage, heal)</t>
+  </si>
+  <si>
+    <t>Retrieve other E HEROes</t>
+  </si>
+  <si>
+    <t>Multiple attacks; Spell/Trap negation</t>
+  </si>
+  <si>
+    <t>Support cards / variants</t>
+  </si>
+  <si>
+    <t>Attack target? Destroy both and deal damage; negate attack and Special Summon an E HERO; Spell/Trap Destruction; effect damage</t>
+  </si>
+  <si>
+    <t>Bonus ATK, battle protection; activate Trap from hand; opponent's monster to DEF pos, then swap Bubbleman for another E HERO; destroys the monster that battles it</t>
+  </si>
+  <si>
+    <t>Change battle positions</t>
+  </si>
+  <si>
+    <t>Bonus ATK; Destroyed? Mass Spell/Trap destruction, effect damage</t>
+  </si>
+  <si>
+    <t>Monster destruction, effect damage</t>
+  </si>
+  <si>
+    <t>Mudballman: LV6, 1900 ATK / 3000 DEF</t>
+  </si>
+  <si>
+    <t>LV3, 1000 ATK / 1000 DEF</t>
+  </si>
+  <si>
+    <t>LV3, 1200 ATK / 800 DEF</t>
+  </si>
+  <si>
+    <t>LV3, 800 ATK / 2000 DEF</t>
+  </si>
+  <si>
+    <t>LV4, 800 ATK / 1200 DEF, Special Summon, draw cards on Summon</t>
+  </si>
+  <si>
+    <t>LV4, 1600 ATK / 1400 DEF</t>
+  </si>
+  <si>
+    <t>LV4, 1500 ATK / 1600 DEF, Unaffected by Traps</t>
+  </si>
+  <si>
+    <t>LV7, 2600 ATK / 1800 DEF, Piercing battle damage</t>
+  </si>
+  <si>
+    <t>Plasma Vice: LV8, 2600 ATK / 2300 DEF, Piercing battle damage, monster destruction</t>
+  </si>
+  <si>
+    <t>Rampart Blaster: LV6, 2000 ATK / 2500 DEF, safe battle damage</t>
+  </si>
+  <si>
+    <t>Wildwingman: LV8, 1900 ATK / 2300 DEF, Spell/Trap destruction</t>
+  </si>
+  <si>
+    <t>Wildedge: LV8, 2600 ATK / 2300 DEF, multiple attacks</t>
+  </si>
+  <si>
+    <t>LV8, 2600 ATK / 2300 DEF, Maximise battle damage</t>
+  </si>
+  <si>
+    <t>Mariner: LV5, 1400 ATK / 1000 DEF, direct attacker</t>
+  </si>
+  <si>
+    <t>Steam Healer: LV5, 1800 ATK / 1000 DEF, LP gain</t>
+  </si>
+  <si>
+    <t>LV8, 2500 ATK / 2100 DEF, indestructible by battle, gains ATK for each E HERO in GY</t>
+  </si>
+  <si>
+    <t>Phoenix Enforcer: LV6, 2100 ATK / 1200 DEF, indestructible by battle</t>
+  </si>
+  <si>
+    <t>Flame Wingman: LV6, 2100 ATK / 1200 DEF, bonus damage after battle</t>
+  </si>
+  <si>
+    <t>LV8, 2800 ATK / 2800 DEF, makes a monster indestructible by battle</t>
+  </si>
+  <si>
+    <t>LV10, 2900 ATK / 2600 DEF, multiple Attributes, recover banished cards, gains ATK for each opponent's monster with the same Attribute</t>
+  </si>
+  <si>
+    <t>LV8, 2500 ATK / 2100 DEF, gains ATK for each E HERO in GY, deals bonus damage after battle</t>
+  </si>
+  <si>
+    <t>Thunder Giant: LV6, 2400 ATK, 1500 DEF, monster destruction</t>
+  </si>
+  <si>
+    <t>High DEF (or ATK), make it safer to attack</t>
+  </si>
+  <si>
+    <t>Darkbright: Level 6, 2000 ATK / 1000 DEF, piercing battle damage, to DEF pos after battle, monster destruction when destroyed</t>
+  </si>
+  <si>
+    <t>Necroid Shaman: LV6, 1900 ATK / 1800 DEF, monster destruction, then swaps for different monster in opponent's GY</t>
+  </si>
+  <si>
+    <t>LV5, 1600 ATK / 1800 DEF, Normal Summon without Tribute while in GY, low ATK/DEF</t>
+  </si>
+  <si>
+    <t>Number of 3 card Fusions</t>
+  </si>
+  <si>
+    <t>4 (2 with Avian due to Phoenix Enforcer)</t>
+  </si>
+  <si>
+    <t>4 (2 with Burstinatrix due to Phoenix Enforcer)</t>
+  </si>
+  <si>
+    <t>Tombstone                 Avalanche</t>
+  </si>
+  <si>
+    <t>Ceramic Edge            Alloy</t>
+  </si>
+  <si>
+    <t>Hydro Blade              Mercurial</t>
+  </si>
+  <si>
+    <t>Plasma                   Solar                     Firestorm</t>
+  </si>
+  <si>
+    <t>Electrolosis                     Conduction              Lightning Chain</t>
+  </si>
+  <si>
+    <t>Necroblaze                  Infernal                   Hellfire</t>
+  </si>
+  <si>
+    <t>Forge                           Molten</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,8 +422,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="27">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,6 +640,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF666633"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -419,7 +680,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -446,6 +707,117 @@
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,6 +826,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF666633"/>
       <color rgb="FFFFFF66"/>
       <color rgb="FF00FFFF"/>
     </mruColors>
@@ -768,8 +1141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45DDA580-D540-48ED-A565-4A56EB1FF400}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -785,28 +1158,28 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
         <v>47</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>49</v>
-      </c>
-      <c r="I1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -837,7 +1210,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -851,7 +1224,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -865,7 +1238,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>2</v>
@@ -882,7 +1255,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>3</v>
@@ -902,13 +1275,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
         <v>26</v>
@@ -917,7 +1290,7 @@
         <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" s="25" t="s">
         <v>9</v>
@@ -925,7 +1298,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>5</v>
@@ -943,7 +1316,7 @@
         <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H8" s="25" t="s">
         <v>9</v>
@@ -951,7 +1324,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>6</v>
@@ -980,7 +1353,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>7</v>
@@ -989,10 +1362,10 @@
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="F10" t="s">
         <v>33</v>
@@ -1043,7 +1416,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>4</v>
@@ -1084,4 +1457,527 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5B8DB6-9BFC-4A71-94E0-C441ACE93E9B}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="14.21875" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="6.5546875" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="27" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="27" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="27" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E6AE20-B16C-4F4A-8168-EBC3DC3242E9}">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="18.88671875" customWidth="1"/>
+    <col min="7" max="7" width="17.77734375" customWidth="1"/>
+    <col min="8" max="9" width="18.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="27" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="27" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="27">
+        <v>3</v>
+      </c>
+      <c r="E3" s="27">
+        <v>3</v>
+      </c>
+      <c r="F3" s="27">
+        <v>3</v>
+      </c>
+      <c r="G3" s="27">
+        <v>3</v>
+      </c>
+      <c r="H3" s="27">
+        <v>2</v>
+      </c>
+      <c r="I3" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="27" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="27" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="27" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="27" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="27" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="27" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="51" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="27" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="52" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="27" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="27" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="G14" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="H14" s="45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="27" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="F15" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+    </row>
+    <row r="19" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+    </row>
+    <row r="20" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+    </row>
+    <row r="21" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+    </row>
+    <row r="22" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+    </row>
+    <row r="23" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>